<commit_message>
Small speed and accessibility changes to support a new plugin
</commit_message>
<xml_diff>
--- a/ExcelExamples/PFE.xlsx
+++ b/ExcelExamples/PFE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>CCIRS001_ZAR</t>
+  </si>
+  <si>
+    <t>amounts</t>
+  </si>
+  <si>
+    <t>currencies</t>
+  </si>
+  <si>
+    <t>QSA.CreateCashLeg</t>
+  </si>
+  <si>
+    <t>CCIRS001_NOTIONALS</t>
   </si>
 </sst>
 </file>
@@ -373,184 +385,184 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="81"/>
                 <c:pt idx="0">
-                  <c:v>812470.45115541469</c:v>
+                  <c:v>-247510.45287915369</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>676406.4111330345</c:v>
+                  <c:v>-322473.29444627627</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>620389.56361578591</c:v>
+                  <c:v>-387054.01198156684</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>459865.79414842813</c:v>
+                  <c:v>-376984.88783765247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>411310.11213500251</c:v>
+                  <c:v>-480581.8007061893</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>364460.67104505212</c:v>
+                  <c:v>-572811.02681570232</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>190673.20965152877</c:v>
+                  <c:v>-543401.66666666663</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>164680.76883644651</c:v>
+                  <c:v>-584240.6430738708</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>138866.68670247047</c:v>
+                  <c:v>-598812.65742714994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1279.0000000000045</c:v>
+                  <c:v>-622771.48850902182</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-31042.368421052615</c:v>
+                  <c:v>-656188.8322253878</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-46673.843501326228</c:v>
+                  <c:v>-690455.39728226094</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-141500.73586471617</c:v>
+                  <c:v>-696746.01690814632</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-178245.3009782834</c:v>
+                  <c:v>-724705.45668946649</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-183448.68626744513</c:v>
+                  <c:v>-719197.22705397895</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-271967.90977072308</c:v>
+                  <c:v>-659995.45555201767</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-296362.26340326335</c:v>
+                  <c:v>-649526.56303837488</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-332667.60055266361</c:v>
+                  <c:v>-765543.52428099944</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-436111.12446587841</c:v>
+                  <c:v>-742740.33333333337</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-440278.25362886902</c:v>
+                  <c:v>-720974.4375757575</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-456459.13649451657</c:v>
+                  <c:v>-748377.83870967734</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-551454.58569402201</c:v>
+                  <c:v>-719905.62801932346</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-577314.05205376178</c:v>
+                  <c:v>-715179.97297297278</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-578446.80718722788</c:v>
+                  <c:v>-719739.34285714279</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-674250.50030317425</c:v>
+                  <c:v>-698344.97849462368</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-675210.76000435161</c:v>
+                  <c:v>-669571.62650602404</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-692286.05387205374</c:v>
+                  <c:v>-671691.86440414109</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-644866.29610467085</c:v>
+                  <c:v>-612526.43666061712</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-653586.25492047111</c:v>
+                  <c:v>-667483.16</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-656309.7843193817</c:v>
+                  <c:v>-687457.72352038196</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-605627.97315663821</c:v>
+                  <c:v>-614718.38599714218</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-617098.22014314949</c:v>
+                  <c:v>-612279.82463755272</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-626940.31131729193</c:v>
+                  <c:v>-614780.57819544151</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-564454.7201861724</c:v>
+                  <c:v>-559750.20346320339</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-572852.27246676874</c:v>
+                  <c:v>-565354.99246704334</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-576670.50935391826</c:v>
+                  <c:v>-569595.83950617281</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-513214.83669638581</c:v>
+                  <c:v>-532853.79738562088</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-526920.14285714272</c:v>
+                  <c:v>-524287</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-527642.44319999998</c:v>
+                  <c:v>-526857.03921568627</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-465274.15268909821</c:v>
+                  <c:v>-462804.59393691941</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-478935.38542940898</c:v>
+                  <c:v>-471225.13827592233</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-477186.66181852255</c:v>
+                  <c:v>-482109.02276422753</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-419563.9195186568</c:v>
+                  <c:v>-414343.89739928889</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-424923.07333910582</c:v>
+                  <c:v>-418850.08205484261</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-428340.67348981148</c:v>
+                  <c:v>-408746.70176820882</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-358842.44217666012</c:v>
+                  <c:v>-348599.66313932976</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-364292.90247603314</c:v>
+                  <c:v>-356955.59042033233</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-365948.18823681655</c:v>
+                  <c:v>-359289.74099547509</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-293583.96626550553</c:v>
+                  <c:v>-291529.07404137921</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-295862.78577439836</c:v>
+                  <c:v>-295212.2078654347</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-297513.85286427505</c:v>
+                  <c:v>-290668.1651085756</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-223735.58247721026</c:v>
+                  <c:v>-219998.63728891971</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-225971.80432163455</c:v>
+                  <c:v>-219895.24359913589</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-229053.23194979099</c:v>
+                  <c:v>-216544.73288571008</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-156069.23842164961</c:v>
+                  <c:v>-149251.55111111113</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-156229.94641308603</c:v>
+                  <c:v>-149750.44328767122</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-156367.11548394861</c:v>
+                  <c:v>-143549.17483412873</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-79077.099851947438</c:v>
+                  <c:v>-78142.390966194202</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-78297.658772058916</c:v>
+                  <c:v>-76427.744430900246</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-77820.849008331352</c:v>
+                  <c:v>-77336.809574410392</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>-9.0599060058593746E-7</c:v>
@@ -644,184 +656,184 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="81"/>
                 <c:pt idx="0">
-                  <c:v>840924.38212357298</c:v>
+                  <c:v>-187932.51406398907</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>739914.41555537097</c:v>
+                  <c:v>-242672.15942028986</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>699428.29493415158</c:v>
+                  <c:v>-285397.70967741928</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>537891.50449329009</c:v>
+                  <c:v>-286812.92338482745</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>502699.86259906972</c:v>
+                  <c:v>-379488.23276050546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>458181.1792499203</c:v>
+                  <c:v>-424573.91597773292</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>317789.96412191913</c:v>
+                  <c:v>-434232.52619483724</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>283016.41191086266</c:v>
+                  <c:v>-447860.29263655003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>281636.52563408908</c:v>
+                  <c:v>-471316.72608890885</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>142859.10810810816</c:v>
+                  <c:v>-450999.14035087713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>147307.24089798299</c:v>
+                  <c:v>-471929.92202462378</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>104955.15037593985</c:v>
+                  <c:v>-520765.59974259976</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9411.2105263158228</c:v>
+                  <c:v>-500455.72727272724</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-5827.9230769230571</c:v>
+                  <c:v>-483486.76567195763</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-5850.4285714285625</c:v>
+                  <c:v>-495711.33628023352</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-115529.04077856451</c:v>
+                  <c:v>-496533.62140198977</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-119505.05527101042</c:v>
+                  <c:v>-527146.75272727269</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-161695.86178581673</c:v>
+                  <c:v>-568523.09470512264</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-253233.53071895419</c:v>
+                  <c:v>-524287</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-275539.27756858524</c:v>
+                  <c:v>-517709.76923076925</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-288598.41570716613</c:v>
+                  <c:v>-549182.31182795693</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-377124.46341463417</c:v>
+                  <c:v>-528086.18840579712</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-416329.66712708597</c:v>
+                  <c:v>-560100.01525658811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-416083.53868259361</c:v>
+                  <c:v>-559903.92033057846</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-512580.96529889002</c:v>
+                  <c:v>-528045.33691756264</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-508290.96532195847</c:v>
+                  <c:v>-510823.80197530863</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-508409.61052631569</c:v>
+                  <c:v>-494019.80878431373</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-482065.46627780289</c:v>
+                  <c:v>-486670.17441364605</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-481190.51747543679</c:v>
+                  <c:v>-496332.37853107345</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-478211.71938894264</c:v>
+                  <c:v>-490397.7349824236</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-451317.79383169982</c:v>
+                  <c:v>-465713.76838777662</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-466465.00304666389</c:v>
+                  <c:v>-472333.02686792449</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-470148.71755331615</c:v>
+                  <c:v>-483631.91315136477</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-423127.51605499501</c:v>
+                  <c:v>-415899.45123958169</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-426452.48612561723</c:v>
+                  <c:v>-417172.53067517275</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-441014.12248771562</c:v>
+                  <c:v>-441554.43314368639</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-392767.43581798801</c:v>
+                  <c:v>-382837.6080877115</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-402126.16935147333</c:v>
+                  <c:v>-379132.53499115095</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-403731.38446724153</c:v>
+                  <c:v>-408039.53454099665</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-360665.14036341087</c:v>
+                  <c:v>-366351.09217502235</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-365428.52531425148</c:v>
+                  <c:v>-354618.38767310086</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-370669.38595327636</c:v>
+                  <c:v>-351807.78601397556</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-323186.72205706756</c:v>
+                  <c:v>-311630.33186813188</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-322722.56516407721</c:v>
+                  <c:v>-313257.04484226136</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-325484.13509920478</c:v>
+                  <c:v>-321443.82350282476</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-274515.95226858585</c:v>
+                  <c:v>-274180.22448979586</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-277401.00822464231</c:v>
+                  <c:v>-275382.59595959593</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-280486.2456519971</c:v>
+                  <c:v>-274600.08287999994</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-226288.61963605581</c:v>
+                  <c:v>-220332.36105763057</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-225771.7186991323</c:v>
+                  <c:v>-218341.63314870396</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-226040.04420882842</c:v>
+                  <c:v>-220581.85535351199</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-169862.14692181698</c:v>
+                  <c:v>-167099.70174132992</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-173050.0674084631</c:v>
+                  <c:v>-171895.2090516552</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-172943.31580858704</c:v>
+                  <c:v>-170139.46859083191</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-116261.46376054977</c:v>
+                  <c:v>-116688.55913495259</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-116607.48258555957</c:v>
+                  <c:v>-115133.26848880966</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-116820.97899351713</c:v>
+                  <c:v>-116115.59317815838</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-58899.797859627593</c:v>
+                  <c:v>-59196.581550430674</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-59149.137977818515</c:v>
+                  <c:v>-58132.551835105682</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-58620.131202674951</c:v>
+                  <c:v>-58329.421335658742</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>-8.5830688476562502E-7</c:v>
@@ -915,184 +927,184 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="81"/>
                 <c:pt idx="0">
-                  <c:v>1038956.976802166</c:v>
+                  <c:v>223192.90458982016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1126390.069304869</c:v>
+                  <c:v>293234.93147343886</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1168506.7974617232</c:v>
+                  <c:v>307015.6274160833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1104841.3477910031</c:v>
+                  <c:v>322990.56183255359</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1126449.092516646</c:v>
+                  <c:v>353039.05280528055</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1172833.393323235</c:v>
+                  <c:v>411969.20023818978</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1064064.2448842255</c:v>
+                  <c:v>413149.19403462228</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1102233.8144639777</c:v>
+                  <c:v>480905.42174482171</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1106532.4348232956</c:v>
+                  <c:v>447737.05256279942</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1005412.5734108672</c:v>
+                  <c:v>497959.04976967996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1033530.6850703455</c:v>
+                  <c:v>498492.70256410254</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1049294.4570858283</c:v>
+                  <c:v>498672.83707233134</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>928535.65751721873</c:v>
+                  <c:v>500134.97779591836</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>931434.88820600521</c:v>
+                  <c:v>536691.00871459697</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>947783.77084090386</c:v>
+                  <c:v>558126.37267670606</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>820350.98218042171</c:v>
+                  <c:v>541588.17976499698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>838431.36850625626</c:v>
+                  <c:v>570196.05757648614</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>860113.98099408508</c:v>
+                  <c:v>572040.71034482773</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>739437.45989397948</c:v>
+                  <c:v>550447.90122448979</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>733643.76394354552</c:v>
+                  <c:v>529891.63362487848</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>754132.1629776737</c:v>
+                  <c:v>551250.38285714295</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>626726.11599060567</c:v>
+                  <c:v>515546.49314138253</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>649318.36739099026</c:v>
+                  <c:v>537264.42574257427</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>661357.07371007383</c:v>
+                  <c:v>547190.3694207028</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>517660.79779311235</c:v>
+                  <c:v>519262.78862135095</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>527484.09197979083</c:v>
+                  <c:v>508642.02691710211</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>544618.18013292085</c:v>
+                  <c:v>542128.23076923063</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>504862.83348840295</c:v>
+                  <c:v>496250.20855614974</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>511731.0398608151</c:v>
+                  <c:v>493188.3073724095</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>519625.16944087821</c:v>
+                  <c:v>496917.22229241795</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>487484.36020991579</c:v>
+                  <c:v>463029.16941187275</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>495957.24211420794</c:v>
+                  <c:v>463805.72428987018</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>504184.53535353555</c:v>
+                  <c:v>480443.51675075572</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>448541.49445160746</c:v>
+                  <c:v>428184.94306763256</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>456159.47380619089</c:v>
+                  <c:v>426617.78678959043</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>465507.88678652374</c:v>
+                  <c:v>431772.26560977229</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>412883.73234966345</c:v>
+                  <c:v>412595.80626341864</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>412863.0723327414</c:v>
+                  <c:v>404922.13135709817</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>418324.23552235152</c:v>
+                  <c:v>428218.2114628409</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>375385.49981050246</c:v>
+                  <c:v>380714.99629554438</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>376412.75229356857</c:v>
+                  <c:v>391131.89142857149</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>379499.48769969417</c:v>
+                  <c:v>399181.59614896105</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>325320.27229233511</c:v>
+                  <c:v>333495.33671836747</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>326818.79119199753</c:v>
+                  <c:v>334342.57798861491</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>335078.45678911702</c:v>
+                  <c:v>350042.86067491584</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>279095.89458434808</c:v>
+                  <c:v>287541.97753613204</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>276561.5847123721</c:v>
+                  <c:v>286786.30043076928</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>279200.47323393961</c:v>
+                  <c:v>277645.78605604917</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>226682.88887811842</c:v>
+                  <c:v>233705.81323924186</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>229443.84698843717</c:v>
+                  <c:v>241290.66421692376</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>231605.42571368814</c:v>
+                  <c:v>236545.43571543644</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>174827.99434760681</c:v>
+                  <c:v>183336.3855584416</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>174797.32077038143</c:v>
+                  <c:v>180778.47319893009</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>175046.58172475666</c:v>
+                  <c:v>181591.96504820333</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>119492.44052253169</c:v>
+                  <c:v>121201.97491787438</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>120247.33514695955</c:v>
+                  <c:v>120272.55846514797</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>118784.3791641854</c:v>
+                  <c:v>122696.49642707019</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>59898.547642976991</c:v>
+                  <c:v>60716.905674653215</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>59810.893342545322</c:v>
+                  <c:v>60989.619384388861</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>59917.543758596563</c:v>
+                  <c:v>62993.262140094543</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
@@ -1186,184 +1198,184 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="81"/>
                 <c:pt idx="0">
-                  <c:v>1067795.7542391585</c:v>
+                  <c:v>280744.15968218364</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1172528.5844982974</c:v>
+                  <c:v>355083.8798336797</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1223025.3810966988</c:v>
+                  <c:v>364454.62983003812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1178235.5011371688</c:v>
+                  <c:v>390877.7842293905</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1211401.5173159167</c:v>
+                  <c:v>435165.55633708154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1261603.2394010345</c:v>
+                  <c:v>475473.07464480028</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1170569.2573791135</c:v>
+                  <c:v>489093.82960413082</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1214025.9992790096</c:v>
+                  <c:v>578001.40254636726</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1214593.4856366054</c:v>
+                  <c:v>589284.55130851059</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1118808.1964869264</c:v>
+                  <c:v>601743.86287260195</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1144615.777746751</c:v>
+                  <c:v>630209.20689655142</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1172342.9939541661</c:v>
+                  <c:v>658952.28573268419</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1043505.4338252763</c:v>
+                  <c:v>622522.57473897806</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1069824.6793536129</c:v>
+                  <c:v>676372.3275503749</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1095349.0441493019</c:v>
+                  <c:v>666258.75509011396</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>963874.97229360591</c:v>
+                  <c:v>649103.69228696311</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>985612.51450215222</c:v>
+                  <c:v>682177.90119674522</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>995010.32435368933</c:v>
+                  <c:v>687978.62521769409</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>859184.46693424275</c:v>
+                  <c:v>661115.22153731994</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>871150.23780549364</c:v>
+                  <c:v>666531.20597981242</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>892518.4986841575</c:v>
+                  <c:v>671586.96190476185</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>752828.03123287554</c:v>
+                  <c:v>645134.62280492764</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>777782.23656385962</c:v>
+                  <c:v>667038.68316831673</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>785378.65865252609</c:v>
+                  <c:v>646514.76689976687</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>656890.82197117945</c:v>
+                  <c:v>633512.35244606074</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>664213.87762483081</c:v>
+                  <c:v>657051.73513559182</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>680351.5588631758</c:v>
+                  <c:v>670015.91168091143</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>626465.58528132236</c:v>
+                  <c:v>613975.6645284947</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>641921.00339979515</c:v>
+                  <c:v>624574.24841915048</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>646631.98560679774</c:v>
+                  <c:v>622327.7424508261</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>595007.1477973474</c:v>
+                  <c:v>560155.10980392131</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>602718.25814372662</c:v>
+                  <c:v>562575.22509462223</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>613075.05706625606</c:v>
+                  <c:v>593952.6657534244</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>552124.45290344558</c:v>
+                  <c:v>534849.57875457872</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>560100.56286919757</c:v>
+                  <c:v>542093.00754716981</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>558843.37669481244</c:v>
+                  <c:v>535857.62146892655</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>501217.83958918613</c:v>
+                  <c:v>502973.74854202394</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>504107.47870384034</c:v>
+                  <c:v>510332.01253283297</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>511147.85042880772</c:v>
+                  <c:v>513524.66931147856</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>452270.01099709212</c:v>
+                  <c:v>454660.73362136004</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>461248.55436285364</c:v>
+                  <c:v>463838.59088761895</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>468375.7957679836</c:v>
+                  <c:v>466452.74027613114</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>405314.81119832519</c:v>
+                  <c:v>412236.78684807243</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>407677.15810445178</c:v>
+                  <c:v>409510.39888087485</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>408733.89008042862</c:v>
+                  <c:v>409657.39429743175</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>343327.08354240132</c:v>
+                  <c:v>346161.77685950405</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>348386.80670417967</c:v>
+                  <c:v>348458.28106666659</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>350225.13716598589</c:v>
+                  <c:v>347016.08939014195</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>277713.239865045</c:v>
+                  <c:v>281059.11025447201</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>279983.5071716152</c:v>
+                  <c:v>285183.31412373477</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>282672.91713673802</c:v>
+                  <c:v>289787.05424754717</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>213909.32087979192</c:v>
+                  <c:v>223348.1965550239</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>216490.30133699434</c:v>
+                  <c:v>225003.78241170608</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>218433.44247666642</c:v>
+                  <c:v>219433.71767280236</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>149530.16793565382</c:v>
+                  <c:v>153501.87058823518</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>148414.60598762767</c:v>
+                  <c:v>154421.58672283357</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>150604.8187686828</c:v>
+                  <c:v>153118.79240037061</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>75653.498129823725</c:v>
+                  <c:v>78212.777777777737</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>74780.478372810248</c:v>
+                  <c:v>78512.653430253471</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>73946.816400460651</c:v>
+                  <c:v>76154.76508166964</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
@@ -1443,11 +1455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="164811136"/>
-        <c:axId val="164812672"/>
+        <c:axId val="377474432"/>
+        <c:axId val="377515008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="164811136"/>
+        <c:axId val="377474432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1456,7 +1468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164812672"/>
+        <c:crossAx val="377515008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1464,7 +1476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164812672"/>
+        <c:axId val="377515008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164811136"/>
+        <c:crossAx val="377474432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1824,14 +1836,15 @@
   <dimension ref="B2:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -1848,24 +1861,29 @@
       </c>
       <c r="C3" s="15" t="str">
         <f>Trades!B10</f>
-        <v>ZARSwap0001.20:17:41-54</v>
+        <v>ZARSwap0001.19:02:17-35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="C4" s="15" t="str">
         <f>Trades!B28</f>
-        <v>CCIRS001_ZAR.20:17:41-55</v>
+        <v>CCIRS001_ZAR.19:02:17-37</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="15" t="str">
         <f>Trades!H28</f>
-        <v>CCIRS001_USD.20:17:41-56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>CCIRS001_USD.19:02:17-36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="str">
+        <f>Trades!N23</f>
+        <v>CCIRS001_NOTIONALS.19:02:17-44</v>
+      </c>
+    </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>39</v>
@@ -1880,8 +1898,8 @@
         <v>40</v>
       </c>
       <c r="C8" s="15" t="str">
-        <f>'Whole Model'!B11</f>
-        <v>fxAndRateModel.20:17:41-63</v>
+        <f ca="1">'Whole Model'!B11</f>
+        <v>fxAndRateModel.19:02:17-45</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1889,7 +1907,7 @@
         <v>41</v>
       </c>
       <c r="C9" s="13">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1929,20 +1947,20 @@
         <v>42676</v>
       </c>
       <c r="C13" s="21">
-        <f t="array" aca="1" ref="C13:F93" ca="1">_xll.QSA.PFE(C3:C5,C7,B13:B93,C10:F10,C8,C9)</f>
-        <v>812470.45115541469</v>
+        <f t="array" aca="1" ref="C13:F93" ca="1">_xll.QSA.PFE(C3,C7,B13:B93,C10:F10,C8,C9)</f>
+        <v>-247510.45287915369</v>
       </c>
       <c r="D13" s="21">
         <f ca="1"/>
-        <v>840924.38212357298</v>
+        <v>-187932.51406398907</v>
       </c>
       <c r="E13" s="21">
         <f ca="1"/>
-        <v>1038956.976802166</v>
+        <v>223192.90458982016</v>
       </c>
       <c r="F13" s="21">
         <f ca="1"/>
-        <v>1067795.7542391585</v>
+        <v>280744.15968218364</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1952,19 +1970,19 @@
       </c>
       <c r="C14" s="21">
         <f ca="1"/>
-        <v>676406.4111330345</v>
+        <v>-322473.29444627627</v>
       </c>
       <c r="D14" s="21">
         <f ca="1"/>
-        <v>739914.41555537097</v>
+        <v>-242672.15942028986</v>
       </c>
       <c r="E14" s="21">
         <f ca="1"/>
-        <v>1126390.069304869</v>
+        <v>293234.93147343886</v>
       </c>
       <c r="F14" s="21">
         <f ca="1"/>
-        <v>1172528.5844982974</v>
+        <v>355083.8798336797</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1974,19 +1992,19 @@
       </c>
       <c r="C15" s="21">
         <f ca="1"/>
-        <v>620389.56361578591</v>
+        <v>-387054.01198156684</v>
       </c>
       <c r="D15" s="21">
         <f ca="1"/>
-        <v>699428.29493415158</v>
+        <v>-285397.70967741928</v>
       </c>
       <c r="E15" s="21">
         <f ca="1"/>
-        <v>1168506.7974617232</v>
+        <v>307015.6274160833</v>
       </c>
       <c r="F15" s="21">
         <f ca="1"/>
-        <v>1223025.3810966988</v>
+        <v>364454.62983003812</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1996,19 +2014,19 @@
       </c>
       <c r="C16" s="21">
         <f ca="1"/>
-        <v>459865.79414842813</v>
+        <v>-376984.88783765247</v>
       </c>
       <c r="D16" s="21">
         <f ca="1"/>
-        <v>537891.50449329009</v>
+        <v>-286812.92338482745</v>
       </c>
       <c r="E16" s="21">
         <f ca="1"/>
-        <v>1104841.3477910031</v>
+        <v>322990.56183255359</v>
       </c>
       <c r="F16" s="21">
         <f ca="1"/>
-        <v>1178235.5011371688</v>
+        <v>390877.7842293905</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2018,19 +2036,19 @@
       </c>
       <c r="C17" s="21">
         <f ca="1"/>
-        <v>411310.11213500251</v>
+        <v>-480581.8007061893</v>
       </c>
       <c r="D17" s="21">
         <f ca="1"/>
-        <v>502699.86259906972</v>
+        <v>-379488.23276050546</v>
       </c>
       <c r="E17" s="21">
         <f ca="1"/>
-        <v>1126449.092516646</v>
+        <v>353039.05280528055</v>
       </c>
       <c r="F17" s="21">
         <f ca="1"/>
-        <v>1211401.5173159167</v>
+        <v>435165.55633708154</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -2040,19 +2058,19 @@
       </c>
       <c r="C18" s="21">
         <f ca="1"/>
-        <v>364460.67104505212</v>
+        <v>-572811.02681570232</v>
       </c>
       <c r="D18" s="21">
         <f ca="1"/>
-        <v>458181.1792499203</v>
+        <v>-424573.91597773292</v>
       </c>
       <c r="E18" s="21">
         <f ca="1"/>
-        <v>1172833.393323235</v>
+        <v>411969.20023818978</v>
       </c>
       <c r="F18" s="21">
         <f ca="1"/>
-        <v>1261603.2394010345</v>
+        <v>475473.07464480028</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -2062,19 +2080,19 @@
       </c>
       <c r="C19" s="21">
         <f ca="1"/>
-        <v>190673.20965152877</v>
+        <v>-543401.66666666663</v>
       </c>
       <c r="D19" s="21">
         <f ca="1"/>
-        <v>317789.96412191913</v>
+        <v>-434232.52619483724</v>
       </c>
       <c r="E19" s="21">
         <f ca="1"/>
-        <v>1064064.2448842255</v>
+        <v>413149.19403462228</v>
       </c>
       <c r="F19" s="21">
         <f ca="1"/>
-        <v>1170569.2573791135</v>
+        <v>489093.82960413082</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2084,19 +2102,19 @@
       </c>
       <c r="C20" s="21">
         <f ca="1"/>
-        <v>164680.76883644651</v>
+        <v>-584240.6430738708</v>
       </c>
       <c r="D20" s="21">
         <f ca="1"/>
-        <v>283016.41191086266</v>
+        <v>-447860.29263655003</v>
       </c>
       <c r="E20" s="21">
         <f ca="1"/>
-        <v>1102233.8144639777</v>
+        <v>480905.42174482171</v>
       </c>
       <c r="F20" s="21">
         <f ca="1"/>
-        <v>1214025.9992790096</v>
+        <v>578001.40254636726</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2106,19 +2124,19 @@
       </c>
       <c r="C21" s="21">
         <f ca="1"/>
-        <v>138866.68670247047</v>
+        <v>-598812.65742714994</v>
       </c>
       <c r="D21" s="21">
         <f ca="1"/>
-        <v>281636.52563408908</v>
+        <v>-471316.72608890885</v>
       </c>
       <c r="E21" s="21">
         <f ca="1"/>
-        <v>1106532.4348232956</v>
+        <v>447737.05256279942</v>
       </c>
       <c r="F21" s="21">
         <f ca="1"/>
-        <v>1214593.4856366054</v>
+        <v>589284.55130851059</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -2128,19 +2146,19 @@
       </c>
       <c r="C22" s="21">
         <f ca="1"/>
-        <v>1279.0000000000045</v>
+        <v>-622771.48850902182</v>
       </c>
       <c r="D22" s="21">
         <f ca="1"/>
-        <v>142859.10810810816</v>
+        <v>-450999.14035087713</v>
       </c>
       <c r="E22" s="21">
         <f ca="1"/>
-        <v>1005412.5734108672</v>
+        <v>497959.04976967996</v>
       </c>
       <c r="F22" s="21">
         <f ca="1"/>
-        <v>1118808.1964869264</v>
+        <v>601743.86287260195</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -2150,19 +2168,19 @@
       </c>
       <c r="C23" s="21">
         <f ca="1"/>
-        <v>-31042.368421052615</v>
+        <v>-656188.8322253878</v>
       </c>
       <c r="D23" s="21">
         <f ca="1"/>
-        <v>147307.24089798299</v>
+        <v>-471929.92202462378</v>
       </c>
       <c r="E23" s="21">
         <f ca="1"/>
-        <v>1033530.6850703455</v>
+        <v>498492.70256410254</v>
       </c>
       <c r="F23" s="21">
         <f ca="1"/>
-        <v>1144615.777746751</v>
+        <v>630209.20689655142</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -2172,19 +2190,19 @@
       </c>
       <c r="C24" s="21">
         <f ca="1"/>
-        <v>-46673.843501326228</v>
+        <v>-690455.39728226094</v>
       </c>
       <c r="D24" s="21">
         <f ca="1"/>
-        <v>104955.15037593985</v>
+        <v>-520765.59974259976</v>
       </c>
       <c r="E24" s="21">
         <f ca="1"/>
-        <v>1049294.4570858283</v>
+        <v>498672.83707233134</v>
       </c>
       <c r="F24" s="21">
         <f ca="1"/>
-        <v>1172342.9939541661</v>
+        <v>658952.28573268419</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2194,19 +2212,19 @@
       </c>
       <c r="C25" s="21">
         <f ca="1"/>
-        <v>-141500.73586471617</v>
+        <v>-696746.01690814632</v>
       </c>
       <c r="D25" s="21">
         <f ca="1"/>
-        <v>9411.2105263158228</v>
+        <v>-500455.72727272724</v>
       </c>
       <c r="E25" s="21">
         <f ca="1"/>
-        <v>928535.65751721873</v>
+        <v>500134.97779591836</v>
       </c>
       <c r="F25" s="21">
         <f ca="1"/>
-        <v>1043505.4338252763</v>
+        <v>622522.57473897806</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -2216,19 +2234,19 @@
       </c>
       <c r="C26" s="21">
         <f ca="1"/>
-        <v>-178245.3009782834</v>
+        <v>-724705.45668946649</v>
       </c>
       <c r="D26" s="21">
         <f ca="1"/>
-        <v>-5827.9230769230571</v>
+        <v>-483486.76567195763</v>
       </c>
       <c r="E26" s="21">
         <f ca="1"/>
-        <v>931434.88820600521</v>
+        <v>536691.00871459697</v>
       </c>
       <c r="F26" s="21">
         <f ca="1"/>
-        <v>1069824.6793536129</v>
+        <v>676372.3275503749</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -2238,19 +2256,19 @@
       </c>
       <c r="C27" s="21">
         <f ca="1"/>
-        <v>-183448.68626744513</v>
+        <v>-719197.22705397895</v>
       </c>
       <c r="D27" s="21">
         <f ca="1"/>
-        <v>-5850.4285714285625</v>
+        <v>-495711.33628023352</v>
       </c>
       <c r="E27" s="21">
         <f ca="1"/>
-        <v>947783.77084090386</v>
+        <v>558126.37267670606</v>
       </c>
       <c r="F27" s="21">
         <f ca="1"/>
-        <v>1095349.0441493019</v>
+        <v>666258.75509011396</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -2260,19 +2278,19 @@
       </c>
       <c r="C28" s="21">
         <f ca="1"/>
-        <v>-271967.90977072308</v>
+        <v>-659995.45555201767</v>
       </c>
       <c r="D28" s="21">
         <f ca="1"/>
-        <v>-115529.04077856451</v>
+        <v>-496533.62140198977</v>
       </c>
       <c r="E28" s="21">
         <f ca="1"/>
-        <v>820350.98218042171</v>
+        <v>541588.17976499698</v>
       </c>
       <c r="F28" s="21">
         <f ca="1"/>
-        <v>963874.97229360591</v>
+        <v>649103.69228696311</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -2282,19 +2300,19 @@
       </c>
       <c r="C29" s="21">
         <f ca="1"/>
-        <v>-296362.26340326335</v>
+        <v>-649526.56303837488</v>
       </c>
       <c r="D29" s="21">
         <f ca="1"/>
-        <v>-119505.05527101042</v>
+        <v>-527146.75272727269</v>
       </c>
       <c r="E29" s="21">
         <f ca="1"/>
-        <v>838431.36850625626</v>
+        <v>570196.05757648614</v>
       </c>
       <c r="F29" s="21">
         <f ca="1"/>
-        <v>985612.51450215222</v>
+        <v>682177.90119674522</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -2304,19 +2322,19 @@
       </c>
       <c r="C30" s="21">
         <f ca="1"/>
-        <v>-332667.60055266361</v>
+        <v>-765543.52428099944</v>
       </c>
       <c r="D30" s="21">
         <f ca="1"/>
-        <v>-161695.86178581673</v>
+        <v>-568523.09470512264</v>
       </c>
       <c r="E30" s="21">
         <f ca="1"/>
-        <v>860113.98099408508</v>
+        <v>572040.71034482773</v>
       </c>
       <c r="F30" s="21">
         <f ca="1"/>
-        <v>995010.32435368933</v>
+        <v>687978.62521769409</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -2326,19 +2344,19 @@
       </c>
       <c r="C31" s="21">
         <f ca="1"/>
-        <v>-436111.12446587841</v>
+        <v>-742740.33333333337</v>
       </c>
       <c r="D31" s="21">
         <f ca="1"/>
-        <v>-253233.53071895419</v>
+        <v>-524287</v>
       </c>
       <c r="E31" s="21">
         <f ca="1"/>
-        <v>739437.45989397948</v>
+        <v>550447.90122448979</v>
       </c>
       <c r="F31" s="21">
         <f ca="1"/>
-        <v>859184.46693424275</v>
+        <v>661115.22153731994</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -2348,19 +2366,19 @@
       </c>
       <c r="C32" s="21">
         <f ca="1"/>
-        <v>-440278.25362886902</v>
+        <v>-720974.4375757575</v>
       </c>
       <c r="D32" s="21">
         <f ca="1"/>
-        <v>-275539.27756858524</v>
+        <v>-517709.76923076925</v>
       </c>
       <c r="E32" s="21">
         <f ca="1"/>
-        <v>733643.76394354552</v>
+        <v>529891.63362487848</v>
       </c>
       <c r="F32" s="21">
         <f ca="1"/>
-        <v>871150.23780549364</v>
+        <v>666531.20597981242</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -2370,19 +2388,19 @@
       </c>
       <c r="C33" s="21">
         <f ca="1"/>
-        <v>-456459.13649451657</v>
+        <v>-748377.83870967734</v>
       </c>
       <c r="D33" s="21">
         <f ca="1"/>
-        <v>-288598.41570716613</v>
+        <v>-549182.31182795693</v>
       </c>
       <c r="E33" s="21">
         <f ca="1"/>
-        <v>754132.1629776737</v>
+        <v>551250.38285714295</v>
       </c>
       <c r="F33" s="21">
         <f ca="1"/>
-        <v>892518.4986841575</v>
+        <v>671586.96190476185</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -2392,19 +2410,19 @@
       </c>
       <c r="C34" s="21">
         <f ca="1"/>
-        <v>-551454.58569402201</v>
+        <v>-719905.62801932346</v>
       </c>
       <c r="D34" s="21">
         <f ca="1"/>
-        <v>-377124.46341463417</v>
+        <v>-528086.18840579712</v>
       </c>
       <c r="E34" s="21">
         <f ca="1"/>
-        <v>626726.11599060567</v>
+        <v>515546.49314138253</v>
       </c>
       <c r="F34" s="21">
         <f ca="1"/>
-        <v>752828.03123287554</v>
+        <v>645134.62280492764</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -2414,19 +2432,19 @@
       </c>
       <c r="C35" s="21">
         <f ca="1"/>
-        <v>-577314.05205376178</v>
+        <v>-715179.97297297278</v>
       </c>
       <c r="D35" s="21">
         <f ca="1"/>
-        <v>-416329.66712708597</v>
+        <v>-560100.01525658811</v>
       </c>
       <c r="E35" s="21">
         <f ca="1"/>
-        <v>649318.36739099026</v>
+        <v>537264.42574257427</v>
       </c>
       <c r="F35" s="21">
         <f ca="1"/>
-        <v>777782.23656385962</v>
+        <v>667038.68316831673</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -2436,19 +2454,19 @@
       </c>
       <c r="C36" s="21">
         <f ca="1"/>
-        <v>-578446.80718722788</v>
+        <v>-719739.34285714279</v>
       </c>
       <c r="D36" s="21">
         <f ca="1"/>
-        <v>-416083.53868259361</v>
+        <v>-559903.92033057846</v>
       </c>
       <c r="E36" s="21">
         <f ca="1"/>
-        <v>661357.07371007383</v>
+        <v>547190.3694207028</v>
       </c>
       <c r="F36" s="21">
         <f ca="1"/>
-        <v>785378.65865252609</v>
+        <v>646514.76689976687</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -2458,19 +2476,19 @@
       </c>
       <c r="C37" s="21">
         <f ca="1"/>
-        <v>-674250.50030317425</v>
+        <v>-698344.97849462368</v>
       </c>
       <c r="D37" s="21">
         <f ca="1"/>
-        <v>-512580.96529889002</v>
+        <v>-528045.33691756264</v>
       </c>
       <c r="E37" s="21">
         <f ca="1"/>
-        <v>517660.79779311235</v>
+        <v>519262.78862135095</v>
       </c>
       <c r="F37" s="21">
         <f ca="1"/>
-        <v>656890.82197117945</v>
+        <v>633512.35244606074</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -2480,19 +2498,19 @@
       </c>
       <c r="C38" s="21">
         <f ca="1"/>
-        <v>-675210.76000435161</v>
+        <v>-669571.62650602404</v>
       </c>
       <c r="D38" s="21">
         <f ca="1"/>
-        <v>-508290.96532195847</v>
+        <v>-510823.80197530863</v>
       </c>
       <c r="E38" s="21">
         <f ca="1"/>
-        <v>527484.09197979083</v>
+        <v>508642.02691710211</v>
       </c>
       <c r="F38" s="21">
         <f ca="1"/>
-        <v>664213.87762483081</v>
+        <v>657051.73513559182</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -2502,19 +2520,19 @@
       </c>
       <c r="C39" s="21">
         <f ca="1"/>
-        <v>-692286.05387205374</v>
+        <v>-671691.86440414109</v>
       </c>
       <c r="D39" s="21">
         <f ca="1"/>
-        <v>-508409.61052631569</v>
+        <v>-494019.80878431373</v>
       </c>
       <c r="E39" s="21">
         <f ca="1"/>
-        <v>544618.18013292085</v>
+        <v>542128.23076923063</v>
       </c>
       <c r="F39" s="21">
         <f ca="1"/>
-        <v>680351.5588631758</v>
+        <v>670015.91168091143</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -2524,19 +2542,19 @@
       </c>
       <c r="C40" s="21">
         <f ca="1"/>
-        <v>-644866.29610467085</v>
+        <v>-612526.43666061712</v>
       </c>
       <c r="D40" s="21">
         <f ca="1"/>
-        <v>-482065.46627780289</v>
+        <v>-486670.17441364605</v>
       </c>
       <c r="E40" s="21">
         <f ca="1"/>
-        <v>504862.83348840295</v>
+        <v>496250.20855614974</v>
       </c>
       <c r="F40" s="21">
         <f ca="1"/>
-        <v>626465.58528132236</v>
+        <v>613975.6645284947</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -2546,19 +2564,19 @@
       </c>
       <c r="C41" s="21">
         <f ca="1"/>
-        <v>-653586.25492047111</v>
+        <v>-667483.16</v>
       </c>
       <c r="D41" s="21">
         <f ca="1"/>
-        <v>-481190.51747543679</v>
+        <v>-496332.37853107345</v>
       </c>
       <c r="E41" s="21">
         <f ca="1"/>
-        <v>511731.0398608151</v>
+        <v>493188.3073724095</v>
       </c>
       <c r="F41" s="21">
         <f ca="1"/>
-        <v>641921.00339979515</v>
+        <v>624574.24841915048</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -2568,19 +2586,19 @@
       </c>
       <c r="C42" s="21">
         <f ca="1"/>
-        <v>-656309.7843193817</v>
+        <v>-687457.72352038196</v>
       </c>
       <c r="D42" s="21">
         <f ca="1"/>
-        <v>-478211.71938894264</v>
+        <v>-490397.7349824236</v>
       </c>
       <c r="E42" s="21">
         <f ca="1"/>
-        <v>519625.16944087821</v>
+        <v>496917.22229241795</v>
       </c>
       <c r="F42" s="21">
         <f ca="1"/>
-        <v>646631.98560679774</v>
+        <v>622327.7424508261</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -2590,19 +2608,19 @@
       </c>
       <c r="C43" s="21">
         <f ca="1"/>
-        <v>-605627.97315663821</v>
+        <v>-614718.38599714218</v>
       </c>
       <c r="D43" s="21">
         <f ca="1"/>
-        <v>-451317.79383169982</v>
+        <v>-465713.76838777662</v>
       </c>
       <c r="E43" s="21">
         <f ca="1"/>
-        <v>487484.36020991579</v>
+        <v>463029.16941187275</v>
       </c>
       <c r="F43" s="21">
         <f ca="1"/>
-        <v>595007.1477973474</v>
+        <v>560155.10980392131</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -2612,19 +2630,19 @@
       </c>
       <c r="C44" s="21">
         <f ca="1"/>
-        <v>-617098.22014314949</v>
+        <v>-612279.82463755272</v>
       </c>
       <c r="D44" s="21">
         <f ca="1"/>
-        <v>-466465.00304666389</v>
+        <v>-472333.02686792449</v>
       </c>
       <c r="E44" s="21">
         <f ca="1"/>
-        <v>495957.24211420794</v>
+        <v>463805.72428987018</v>
       </c>
       <c r="F44" s="21">
         <f ca="1"/>
-        <v>602718.25814372662</v>
+        <v>562575.22509462223</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2634,19 +2652,19 @@
       </c>
       <c r="C45" s="21">
         <f ca="1"/>
-        <v>-626940.31131729193</v>
+        <v>-614780.57819544151</v>
       </c>
       <c r="D45" s="21">
         <f ca="1"/>
-        <v>-470148.71755331615</v>
+        <v>-483631.91315136477</v>
       </c>
       <c r="E45" s="21">
         <f ca="1"/>
-        <v>504184.53535353555</v>
+        <v>480443.51675075572</v>
       </c>
       <c r="F45" s="21">
         <f ca="1"/>
-        <v>613075.05706625606</v>
+        <v>593952.6657534244</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -2656,19 +2674,19 @@
       </c>
       <c r="C46" s="21">
         <f ca="1"/>
-        <v>-564454.7201861724</v>
+        <v>-559750.20346320339</v>
       </c>
       <c r="D46" s="21">
         <f ca="1"/>
-        <v>-423127.51605499501</v>
+        <v>-415899.45123958169</v>
       </c>
       <c r="E46" s="21">
         <f ca="1"/>
-        <v>448541.49445160746</v>
+        <v>428184.94306763256</v>
       </c>
       <c r="F46" s="21">
         <f ca="1"/>
-        <v>552124.45290344558</v>
+        <v>534849.57875457872</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2678,19 +2696,19 @@
       </c>
       <c r="C47" s="21">
         <f ca="1"/>
-        <v>-572852.27246676874</v>
+        <v>-565354.99246704334</v>
       </c>
       <c r="D47" s="21">
         <f ca="1"/>
-        <v>-426452.48612561723</v>
+        <v>-417172.53067517275</v>
       </c>
       <c r="E47" s="21">
         <f ca="1"/>
-        <v>456159.47380619089</v>
+        <v>426617.78678959043</v>
       </c>
       <c r="F47" s="21">
         <f ca="1"/>
-        <v>560100.56286919757</v>
+        <v>542093.00754716981</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2700,19 +2718,19 @@
       </c>
       <c r="C48" s="21">
         <f ca="1"/>
-        <v>-576670.50935391826</v>
+        <v>-569595.83950617281</v>
       </c>
       <c r="D48" s="21">
         <f ca="1"/>
-        <v>-441014.12248771562</v>
+        <v>-441554.43314368639</v>
       </c>
       <c r="E48" s="21">
         <f ca="1"/>
-        <v>465507.88678652374</v>
+        <v>431772.26560977229</v>
       </c>
       <c r="F48" s="21">
         <f ca="1"/>
-        <v>558843.37669481244</v>
+        <v>535857.62146892655</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2722,19 +2740,19 @@
       </c>
       <c r="C49" s="21">
         <f ca="1"/>
-        <v>-513214.83669638581</v>
+        <v>-532853.79738562088</v>
       </c>
       <c r="D49" s="21">
         <f ca="1"/>
-        <v>-392767.43581798801</v>
+        <v>-382837.6080877115</v>
       </c>
       <c r="E49" s="21">
         <f ca="1"/>
-        <v>412883.73234966345</v>
+        <v>412595.80626341864</v>
       </c>
       <c r="F49" s="21">
         <f ca="1"/>
-        <v>501217.83958918613</v>
+        <v>502973.74854202394</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2744,19 +2762,19 @@
       </c>
       <c r="C50" s="21">
         <f ca="1"/>
-        <v>-526920.14285714272</v>
+        <v>-524287</v>
       </c>
       <c r="D50" s="21">
         <f ca="1"/>
-        <v>-402126.16935147333</v>
+        <v>-379132.53499115095</v>
       </c>
       <c r="E50" s="21">
         <f ca="1"/>
-        <v>412863.0723327414</v>
+        <v>404922.13135709817</v>
       </c>
       <c r="F50" s="21">
         <f ca="1"/>
-        <v>504107.47870384034</v>
+        <v>510332.01253283297</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -2766,19 +2784,19 @@
       </c>
       <c r="C51" s="21">
         <f ca="1"/>
-        <v>-527642.44319999998</v>
+        <v>-526857.03921568627</v>
       </c>
       <c r="D51" s="21">
         <f ca="1"/>
-        <v>-403731.38446724153</v>
+        <v>-408039.53454099665</v>
       </c>
       <c r="E51" s="21">
         <f ca="1"/>
-        <v>418324.23552235152</v>
+        <v>428218.2114628409</v>
       </c>
       <c r="F51" s="21">
         <f ca="1"/>
-        <v>511147.85042880772</v>
+        <v>513524.66931147856</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -2788,19 +2806,19 @@
       </c>
       <c r="C52" s="21">
         <f ca="1"/>
-        <v>-465274.15268909821</v>
+        <v>-462804.59393691941</v>
       </c>
       <c r="D52" s="21">
         <f ca="1"/>
-        <v>-360665.14036341087</v>
+        <v>-366351.09217502235</v>
       </c>
       <c r="E52" s="21">
         <f ca="1"/>
-        <v>375385.49981050246</v>
+        <v>380714.99629554438</v>
       </c>
       <c r="F52" s="21">
         <f ca="1"/>
-        <v>452270.01099709212</v>
+        <v>454660.73362136004</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -2810,19 +2828,19 @@
       </c>
       <c r="C53" s="21">
         <f ca="1"/>
-        <v>-478935.38542940898</v>
+        <v>-471225.13827592233</v>
       </c>
       <c r="D53" s="21">
         <f ca="1"/>
-        <v>-365428.52531425148</v>
+        <v>-354618.38767310086</v>
       </c>
       <c r="E53" s="21">
         <f ca="1"/>
-        <v>376412.75229356857</v>
+        <v>391131.89142857149</v>
       </c>
       <c r="F53" s="21">
         <f ca="1"/>
-        <v>461248.55436285364</v>
+        <v>463838.59088761895</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
@@ -2832,19 +2850,19 @@
       </c>
       <c r="C54" s="21">
         <f ca="1"/>
-        <v>-477186.66181852255</v>
+        <v>-482109.02276422753</v>
       </c>
       <c r="D54" s="21">
         <f ca="1"/>
-        <v>-370669.38595327636</v>
+        <v>-351807.78601397556</v>
       </c>
       <c r="E54" s="21">
         <f ca="1"/>
-        <v>379499.48769969417</v>
+        <v>399181.59614896105</v>
       </c>
       <c r="F54" s="21">
         <f ca="1"/>
-        <v>468375.7957679836</v>
+        <v>466452.74027613114</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -2854,19 +2872,19 @@
       </c>
       <c r="C55" s="21">
         <f ca="1"/>
-        <v>-419563.9195186568</v>
+        <v>-414343.89739928889</v>
       </c>
       <c r="D55" s="21">
         <f ca="1"/>
-        <v>-323186.72205706756</v>
+        <v>-311630.33186813188</v>
       </c>
       <c r="E55" s="21">
         <f ca="1"/>
-        <v>325320.27229233511</v>
+        <v>333495.33671836747</v>
       </c>
       <c r="F55" s="21">
         <f ca="1"/>
-        <v>405314.81119832519</v>
+        <v>412236.78684807243</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -2876,19 +2894,19 @@
       </c>
       <c r="C56" s="21">
         <f ca="1"/>
-        <v>-424923.07333910582</v>
+        <v>-418850.08205484261</v>
       </c>
       <c r="D56" s="21">
         <f ca="1"/>
-        <v>-322722.56516407721</v>
+        <v>-313257.04484226136</v>
       </c>
       <c r="E56" s="21">
         <f ca="1"/>
-        <v>326818.79119199753</v>
+        <v>334342.57798861491</v>
       </c>
       <c r="F56" s="21">
         <f ca="1"/>
-        <v>407677.15810445178</v>
+        <v>409510.39888087485</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
@@ -2898,19 +2916,19 @@
       </c>
       <c r="C57" s="21">
         <f ca="1"/>
-        <v>-428340.67348981148</v>
+        <v>-408746.70176820882</v>
       </c>
       <c r="D57" s="21">
         <f ca="1"/>
-        <v>-325484.13509920478</v>
+        <v>-321443.82350282476</v>
       </c>
       <c r="E57" s="21">
         <f ca="1"/>
-        <v>335078.45678911702</v>
+        <v>350042.86067491584</v>
       </c>
       <c r="F57" s="21">
         <f ca="1"/>
-        <v>408733.89008042862</v>
+        <v>409657.39429743175</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -2920,19 +2938,19 @@
       </c>
       <c r="C58" s="21">
         <f ca="1"/>
-        <v>-358842.44217666012</v>
+        <v>-348599.66313932976</v>
       </c>
       <c r="D58" s="21">
         <f ca="1"/>
-        <v>-274515.95226858585</v>
+        <v>-274180.22448979586</v>
       </c>
       <c r="E58" s="21">
         <f ca="1"/>
-        <v>279095.89458434808</v>
+        <v>287541.97753613204</v>
       </c>
       <c r="F58" s="21">
         <f ca="1"/>
-        <v>343327.08354240132</v>
+        <v>346161.77685950405</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -2942,19 +2960,19 @@
       </c>
       <c r="C59" s="21">
         <f ca="1"/>
-        <v>-364292.90247603314</v>
+        <v>-356955.59042033233</v>
       </c>
       <c r="D59" s="21">
         <f ca="1"/>
-        <v>-277401.00822464231</v>
+        <v>-275382.59595959593</v>
       </c>
       <c r="E59" s="21">
         <f ca="1"/>
-        <v>276561.5847123721</v>
+        <v>286786.30043076928</v>
       </c>
       <c r="F59" s="21">
         <f ca="1"/>
-        <v>348386.80670417967</v>
+        <v>348458.28106666659</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -2964,19 +2982,19 @@
       </c>
       <c r="C60" s="21">
         <f ca="1"/>
-        <v>-365948.18823681655</v>
+        <v>-359289.74099547509</v>
       </c>
       <c r="D60" s="21">
         <f ca="1"/>
-        <v>-280486.2456519971</v>
+        <v>-274600.08287999994</v>
       </c>
       <c r="E60" s="21">
         <f ca="1"/>
-        <v>279200.47323393961</v>
+        <v>277645.78605604917</v>
       </c>
       <c r="F60" s="21">
         <f ca="1"/>
-        <v>350225.13716598589</v>
+        <v>347016.08939014195</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
@@ -2986,19 +3004,19 @@
       </c>
       <c r="C61" s="21">
         <f ca="1"/>
-        <v>-293583.96626550553</v>
+        <v>-291529.07404137921</v>
       </c>
       <c r="D61" s="21">
         <f ca="1"/>
-        <v>-226288.61963605581</v>
+        <v>-220332.36105763057</v>
       </c>
       <c r="E61" s="21">
         <f ca="1"/>
-        <v>226682.88887811842</v>
+        <v>233705.81323924186</v>
       </c>
       <c r="F61" s="21">
         <f ca="1"/>
-        <v>277713.239865045</v>
+        <v>281059.11025447201</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -3008,19 +3026,19 @@
       </c>
       <c r="C62" s="21">
         <f ca="1"/>
-        <v>-295862.78577439836</v>
+        <v>-295212.2078654347</v>
       </c>
       <c r="D62" s="21">
         <f ca="1"/>
-        <v>-225771.7186991323</v>
+        <v>-218341.63314870396</v>
       </c>
       <c r="E62" s="21">
         <f ca="1"/>
-        <v>229443.84698843717</v>
+        <v>241290.66421692376</v>
       </c>
       <c r="F62" s="21">
         <f ca="1"/>
-        <v>279983.5071716152</v>
+        <v>285183.31412373477</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -3030,19 +3048,19 @@
       </c>
       <c r="C63" s="21">
         <f ca="1"/>
-        <v>-297513.85286427505</v>
+        <v>-290668.1651085756</v>
       </c>
       <c r="D63" s="21">
         <f ca="1"/>
-        <v>-226040.04420882842</v>
+        <v>-220581.85535351199</v>
       </c>
       <c r="E63" s="21">
         <f ca="1"/>
-        <v>231605.42571368814</v>
+        <v>236545.43571543644</v>
       </c>
       <c r="F63" s="21">
         <f ca="1"/>
-        <v>282672.91713673802</v>
+        <v>289787.05424754717</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -3052,19 +3070,19 @@
       </c>
       <c r="C64" s="21">
         <f ca="1"/>
-        <v>-223735.58247721026</v>
+        <v>-219998.63728891971</v>
       </c>
       <c r="D64" s="21">
         <f ca="1"/>
-        <v>-169862.14692181698</v>
+        <v>-167099.70174132992</v>
       </c>
       <c r="E64" s="21">
         <f ca="1"/>
-        <v>174827.99434760681</v>
+        <v>183336.3855584416</v>
       </c>
       <c r="F64" s="21">
         <f ca="1"/>
-        <v>213909.32087979192</v>
+        <v>223348.1965550239</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -3074,19 +3092,19 @@
       </c>
       <c r="C65" s="21">
         <f ca="1"/>
-        <v>-225971.80432163455</v>
+        <v>-219895.24359913589</v>
       </c>
       <c r="D65" s="21">
         <f ca="1"/>
-        <v>-173050.0674084631</v>
+        <v>-171895.2090516552</v>
       </c>
       <c r="E65" s="21">
         <f ca="1"/>
-        <v>174797.32077038143</v>
+        <v>180778.47319893009</v>
       </c>
       <c r="F65" s="21">
         <f ca="1"/>
-        <v>216490.30133699434</v>
+        <v>225003.78241170608</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
@@ -3096,19 +3114,19 @@
       </c>
       <c r="C66" s="21">
         <f ca="1"/>
-        <v>-229053.23194979099</v>
+        <v>-216544.73288571008</v>
       </c>
       <c r="D66" s="21">
         <f ca="1"/>
-        <v>-172943.31580858704</v>
+        <v>-170139.46859083191</v>
       </c>
       <c r="E66" s="21">
         <f ca="1"/>
-        <v>175046.58172475666</v>
+        <v>181591.96504820333</v>
       </c>
       <c r="F66" s="21">
         <f ca="1"/>
-        <v>218433.44247666642</v>
+        <v>219433.71767280236</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
@@ -3118,19 +3136,19 @@
       </c>
       <c r="C67" s="21">
         <f ca="1"/>
-        <v>-156069.23842164961</v>
+        <v>-149251.55111111113</v>
       </c>
       <c r="D67" s="21">
         <f ca="1"/>
-        <v>-116261.46376054977</v>
+        <v>-116688.55913495259</v>
       </c>
       <c r="E67" s="21">
         <f ca="1"/>
-        <v>119492.44052253169</v>
+        <v>121201.97491787438</v>
       </c>
       <c r="F67" s="21">
         <f ca="1"/>
-        <v>149530.16793565382</v>
+        <v>153501.87058823518</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
@@ -3140,19 +3158,19 @@
       </c>
       <c r="C68" s="21">
         <f ca="1"/>
-        <v>-156229.94641308603</v>
+        <v>-149750.44328767122</v>
       </c>
       <c r="D68" s="21">
         <f ca="1"/>
-        <v>-116607.48258555957</v>
+        <v>-115133.26848880966</v>
       </c>
       <c r="E68" s="21">
         <f ca="1"/>
-        <v>120247.33514695955</v>
+        <v>120272.55846514797</v>
       </c>
       <c r="F68" s="21">
         <f ca="1"/>
-        <v>148414.60598762767</v>
+        <v>154421.58672283357</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -3162,19 +3180,19 @@
       </c>
       <c r="C69" s="21">
         <f ca="1"/>
-        <v>-156367.11548394861</v>
+        <v>-143549.17483412873</v>
       </c>
       <c r="D69" s="21">
         <f ca="1"/>
-        <v>-116820.97899351713</v>
+        <v>-116115.59317815838</v>
       </c>
       <c r="E69" s="21">
         <f ca="1"/>
-        <v>118784.3791641854</v>
+        <v>122696.49642707019</v>
       </c>
       <c r="F69" s="21">
         <f ca="1"/>
-        <v>150604.8187686828</v>
+        <v>153118.79240037061</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
@@ -3184,19 +3202,19 @@
       </c>
       <c r="C70" s="21">
         <f ca="1"/>
-        <v>-79077.099851947438</v>
+        <v>-78142.390966194202</v>
       </c>
       <c r="D70" s="21">
         <f ca="1"/>
-        <v>-58899.797859627593</v>
+        <v>-59196.581550430674</v>
       </c>
       <c r="E70" s="21">
         <f ca="1"/>
-        <v>59898.547642976991</v>
+        <v>60716.905674653215</v>
       </c>
       <c r="F70" s="21">
         <f ca="1"/>
-        <v>75653.498129823725</v>
+        <v>78212.777777777737</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
@@ -3206,19 +3224,19 @@
       </c>
       <c r="C71" s="21">
         <f ca="1"/>
-        <v>-78297.658772058916</v>
+        <v>-76427.744430900246</v>
       </c>
       <c r="D71" s="21">
         <f ca="1"/>
-        <v>-59149.137977818515</v>
+        <v>-58132.551835105682</v>
       </c>
       <c r="E71" s="21">
         <f ca="1"/>
-        <v>59810.893342545322</v>
+        <v>60989.619384388861</v>
       </c>
       <c r="F71" s="21">
         <f ca="1"/>
-        <v>74780.478372810248</v>
+        <v>78512.653430253471</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -3228,19 +3246,19 @@
       </c>
       <c r="C72" s="21">
         <f ca="1"/>
-        <v>-77820.849008331352</v>
+        <v>-77336.809574410392</v>
       </c>
       <c r="D72" s="21">
         <f ca="1"/>
-        <v>-58620.131202674951</v>
+        <v>-58329.421335658742</v>
       </c>
       <c r="E72" s="21">
         <f ca="1"/>
-        <v>59917.543758596563</v>
+        <v>62993.262140094543</v>
       </c>
       <c r="F72" s="21">
         <f ca="1"/>
-        <v>73946.816400460651</v>
+        <v>76154.76508166964</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
@@ -3713,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L28"/>
+  <dimension ref="B2:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3731,9 +3749,12 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -3741,7 +3762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
@@ -3749,7 +3770,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
@@ -3757,7 +3778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>32</v>
       </c>
@@ -3765,7 +3786,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -3773,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>34</v>
       </c>
@@ -3781,24 +3802,24 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="str">
         <f>_xll.QSA.CreateZARSwap(C2,C3,C4,C5,C6,C7)</f>
-        <v>ZARSwap0001.20:17:41-54</v>
+        <v>ZARSwap0001.19:02:17-35</v>
       </c>
       <c r="C10" s="9"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>0</v>
       </c>
@@ -3817,8 +3838,15 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>2</v>
       </c>
@@ -3837,8 +3865,11 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>47</v>
       </c>
@@ -3857,8 +3888,17 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -3869,8 +3909,19 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N16" s="16">
+        <f>C25</f>
+        <v>43405</v>
+      </c>
+      <c r="O16" s="18">
+        <f>D25</f>
+        <v>13600000</v>
+      </c>
+      <c r="P16" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>48</v>
       </c>
@@ -3901,8 +3952,19 @@
       <c r="L17" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="16">
+        <f>I25</f>
+        <v>43405</v>
+      </c>
+      <c r="O17" s="18">
+        <f>J25</f>
+        <v>-1000000</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <v>42675</v>
       </c>
@@ -3911,7 +3973,7 @@
         <v>42767</v>
       </c>
       <c r="D18" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E18" s="14">
         <v>0</v>
@@ -3937,8 +3999,12 @@
         <f>(I18-H18)/365</f>
         <v>0.25205479452054796</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <f>C18</f>
         <v>42767</v>
@@ -3948,7 +4014,7 @@
         <v>42856</v>
       </c>
       <c r="D19" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E19" s="14">
         <v>0</v>
@@ -3975,8 +4041,12 @@
         <f t="shared" ref="L19:L25" si="3">(I19-H19)/365</f>
         <v>0.24383561643835616</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <f t="shared" ref="B20:B25" si="4">C19</f>
         <v>42856</v>
@@ -3986,7 +4056,7 @@
         <v>42948</v>
       </c>
       <c r="D20" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E20" s="14">
         <v>0</v>
@@ -4013,8 +4083,11 @@
         <f t="shared" si="3"/>
         <v>0.25205479452054796</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
         <f t="shared" si="4"/>
         <v>42948</v>
@@ -4024,7 +4097,7 @@
         <v>43040</v>
       </c>
       <c r="D21" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E21" s="14">
         <v>0</v>
@@ -4051,8 +4124,11 @@
         <f t="shared" si="3"/>
         <v>0.25205479452054796</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+    </row>
+    <row r="22" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B22" s="16">
         <f t="shared" si="4"/>
         <v>43040</v>
@@ -4062,7 +4138,7 @@
         <v>43132</v>
       </c>
       <c r="D22" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E22" s="14">
         <v>0</v>
@@ -4089,8 +4165,13 @@
         <f t="shared" si="3"/>
         <v>0.25205479452054796</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="16">
         <f t="shared" si="4"/>
         <v>43132</v>
@@ -4100,7 +4181,7 @@
         <v>43221</v>
       </c>
       <c r="D23" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E23" s="14">
         <v>0</v>
@@ -4127,8 +4208,14 @@
         <f t="shared" si="3"/>
         <v>0.24383561643835616</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N23" s="12" t="str">
+        <f>_xll.QSA.CreateCashLeg(O13,N16:N17,O16:O17,P16:P17)</f>
+        <v>CCIRS001_NOTIONALS.19:02:17-44</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <f t="shared" si="4"/>
         <v>43221</v>
@@ -4138,7 +4225,7 @@
         <v>43313</v>
       </c>
       <c r="D24" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E24" s="14">
         <v>0</v>
@@ -4166,7 +4253,7 @@
         <v>0.25205479452054796</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <f t="shared" si="4"/>
         <v>43313</v>
@@ -4176,7 +4263,7 @@
         <v>43405</v>
       </c>
       <c r="D25" s="18">
-        <v>10000000</v>
+        <v>13600000</v>
       </c>
       <c r="E25" s="14">
         <v>0</v>
@@ -4204,7 +4291,7 @@
         <v>0.25205479452054796</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="9"/>
@@ -4216,7 +4303,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="2:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B27" s="10" t="s">
         <v>53</v>
       </c>
@@ -4232,10 +4319,10 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="str">
         <f>_xll.QSA.CreateFloatLeg(C13,C14,C15,B18:B25,C18:C25,D18:D25,E18:E25,F18:F25)</f>
-        <v>CCIRS001_ZAR.20:17:41-55</v>
+        <v>CCIRS001_ZAR.19:02:17-37</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -4243,7 +4330,7 @@
       <c r="F28" s="9"/>
       <c r="H28" s="12" t="str">
         <f>_xll.QSA.CreateFloatLeg(I13,I14,I15,H18:H25,I18:I25,J18:J25,K18:K25,L18:L25)</f>
-        <v>CCIRS001_USD.20:17:41-56</v>
+        <v>CCIRS001_USD.19:02:17-36</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -4260,7 +4347,7 @@
   <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4351,19 +4438,19 @@
       </c>
       <c r="C5" s="15" t="str">
         <f>'HW Models'!B9</f>
-        <v>HWZAR.20:17:41-60</v>
+        <v>HWZAR.19:02:17-42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="str">
-        <f>'HW Models'!B19</f>
-        <v>HWUSD.20:17:41-61</v>
+        <f ca="1">'HW Models'!B19</f>
+        <v>HWUSD.19:02:17-41</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="str">
-        <f>'HW Models'!B29</f>
-        <v>HWEUR.20:17:41-62</v>
+        <f ca="1">'HW Models'!B29</f>
+        <v>HWEUR.19:02:17-43</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
@@ -4373,8 +4460,8 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="str">
-        <f>_xll.QSA.CreateMultiHWAndFXToy(C2,C3,C4,C5:C7,E3:E4,F3:F4,G3:G4,I3:J4)</f>
-        <v>fxAndRateModel.20:17:41-63</v>
+        <f ca="1">_xll.QSA.CreateMultiHWAndFXToy(C2,C3,C4,C5:C7,E3:E4,F3:F4,G3:G4,I3:J4)</f>
+        <v>fxAndRateModel.19:02:17-45</v>
       </c>
     </row>
   </sheetData>
@@ -4387,7 +4474,7 @@
   <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4448,7 +4535,7 @@
       </c>
       <c r="C5" s="7" t="str">
         <f>G9</f>
-        <v>ZARSwapCurve.20:17:41-58</v>
+        <v>ZARSwapCurve.19:02:17-39</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4500,7 +4587,7 @@
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>_xll.QSA.CreateHWModelDemo(C2,C3,C4,C5,C6)</f>
-        <v>HWZAR.20:17:41-60</v>
+        <v>HWZAR.19:02:17-42</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -4508,7 +4595,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="4" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(G2,F6:F7,G6:G7,G3)</f>
-        <v>ZARSwapCurve.20:17:41-58</v>
+        <v>ZARSwapCurve.19:02:17-39</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -4561,7 +4648,7 @@
       </c>
       <c r="C15" s="15" t="str">
         <f>G19</f>
-        <v>USDSwapCurve.20:17:41-57</v>
+        <v>USDSwapCurve.19:02:17-40</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -4612,8 +4699,8 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="str">
-        <f>_xll.QSA.CreateHWModelDemo(C12,C13,C14,C15,C16)</f>
-        <v>HWUSD.20:17:41-61</v>
+        <f ca="1">_xll.QSA.CreateHWModelDemo(C12,C13,C14,C15,C16)</f>
+        <v>HWUSD.19:02:17-41</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -4621,7 +4708,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="12" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(G12,F16:F17,G16:G17,G13)</f>
-        <v>USDSwapCurve.20:17:41-57</v>
+        <v>USDSwapCurve.19:02:17-40</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -4674,7 +4761,7 @@
       </c>
       <c r="C25" s="15" t="str">
         <f>G29</f>
-        <v>EURSwapCurve.20:17:41-59</v>
+        <v>EURSwapCurve.19:02:17-38</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -4725,8 +4812,8 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="str">
-        <f>_xll.QSA.CreateHWModelDemo(C22,C23,C24,C25,C26)</f>
-        <v>HWEUR.20:17:41-62</v>
+        <f ca="1">_xll.QSA.CreateHWModelDemo(C22,C23,C24,C25,C26)</f>
+        <v>HWEUR.19:02:17-43</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -4734,7 +4821,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="12" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(G22,F26:F27,G26:G27,G23)</f>
-        <v>EURSwapCurve.20:17:41-59</v>
+        <v>EURSwapCurve.19:02:17-38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>